<commit_message>
updates for money analysis
</commit_message>
<xml_diff>
--- a/Interpolat_Diff_Tax/Money_Analysis/chinese_price_scaling.xlsx
+++ b/Interpolat_Diff_Tax/Money_Analysis/chinese_price_scaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorgan/Documents/PostDoc/Diff_Tax_Analysis/Theoretical_Analysis/Interpolat_Diff_Tax/Money_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616AAD0B-AF8C-A749-9FF7-625BF3A26444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34C99E3-B417-D94D-B797-E9DB1F6745C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="760" windowWidth="15060" windowHeight="14140" xr2:uid="{41DE4A9E-354A-C947-8AF3-BFD4A954794B}"/>
+    <workbookView xWindow="100" yWindow="580" windowWidth="26520" windowHeight="14140" xr2:uid="{41DE4A9E-354A-C947-8AF3-BFD4A954794B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Antibiotic Class</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Price8</t>
+  </si>
+  <si>
+    <t>Cephalosporins</t>
+  </si>
+  <si>
+    <t>average_price</t>
   </si>
 </sst>
 </file>
@@ -175,7 +181,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -463,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BD6BD6-5BEF-9C4F-865E-676CD3C4F9B8}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +611,7 @@
         <v>453.53999999999996</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f>J4*0.15</f>
         <v>68.030999999999992</v>
       </c>
       <c r="L4">
@@ -751,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="K10">
-        <v>10.894457454330663</v>
+        <v>9.8428938354397566</v>
       </c>
       <c r="L10">
         <v>292.47699999999998</v>
@@ -772,23 +778,68 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="L11">
+        <f>J11*I18</f>
+        <v>2165.4366437967465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>540</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>433.33330000000001</v>
+      </c>
+      <c r="E12">
+        <v>500</v>
+      </c>
+      <c r="J12">
+        <f>AVERAGE(B12:E12)</f>
+        <v>618.33332500000006</v>
+      </c>
+      <c r="K12">
+        <f>J12*0.15</f>
+        <v>92.749998750000003</v>
+      </c>
+      <c r="L12">
+        <v>18964.994444444445</v>
+      </c>
+      <c r="M12">
+        <f>K12/L12</f>
+        <v>4.8905892918502773E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>19</v>
       </c>
       <c r="I16">
-        <f>AVERAGE(M2:M9)</f>
-        <v>3.7248937367145671E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.2">
+        <f>AVERAGE(M2:M12)</f>
+        <v>3.3653565358779516E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17">
+        <f>AVERAGE(K2:K12)</f>
+        <v>50.774878871403615</v>
+      </c>
+    </row>
+    <row r="18" spans="7:13" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>20</v>
       </c>
       <c r="I18">
         <f>L10*I16</f>
-        <v>10.894457454330663</v>
+        <v>9.8428938354397566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>